<commit_message>
jun  12-18  function update
</commit_message>
<xml_diff>
--- a/WebRoot/sqlFile/前台功能请求.xlsx
+++ b/WebRoot/sqlFile/前台功能请求.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="veryHidden" xWindow="0" yWindow="0" windowWidth="15000" windowHeight="6765" tabRatio="781" activeTab="1"/>
+    <workbookView visibility="veryHidden" xWindow="0" yWindow="0" windowWidth="15000" windowHeight="3690" tabRatio="781" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="发送短信" sheetId="1" r:id="rId1"/>
@@ -15,12 +15,12 @@
     <sheet name="获取用户信息" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:L24"/>
+  <oleSize ref="A1:M13"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="45">
   <si>
     <t>功能名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -172,15 +172,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>message=“success” +发送成功数量</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>findAllUser</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>无</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>result</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>result</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1  ： list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>msggroupList</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1+msggroupList</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -533,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5:H5"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15:K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -690,6 +706,11 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
+    <row r="12" spans="1:11">
+      <c r="H12" t="s">
+        <v>41</v>
+      </c>
+    </row>
     <row r="13" spans="1:11">
       <c r="A13" s="2" t="s">
         <v>9</v>
@@ -703,7 +724,7 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -720,8 +741,8 @@
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="2" t="s">
-        <v>12</v>
+      <c r="F14" s="2">
+        <v>0</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -739,9 +760,7 @@
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -758,9 +777,7 @@
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -848,8 +865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13:J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -892,7 +909,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -989,7 +1006,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -1013,8 +1030,8 @@
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="2" t="s">
-        <v>26</v>
+      <c r="F13" s="2">
+        <v>1</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -1022,7 +1039,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="1"/>
       <c r="L13" s="2" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -1037,8 +1054,8 @@
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="2" t="s">
-        <v>12</v>
+      <c r="F14" s="2">
+        <v>0</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -1059,9 +1076,7 @@
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -1081,9 +1096,7 @@
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -1205,8 +1218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15:K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1366,7 +1379,7 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -1374,7 +1387,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="1"/>
       <c r="L13" s="2" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -1389,8 +1402,8 @@
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="2" t="s">
-        <v>12</v>
+      <c r="F14" s="2">
+        <v>0</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -1411,9 +1424,7 @@
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>

</xml_diff>